<commit_message>
add convert idx and readme
</commit_message>
<xml_diff>
--- a/test/excel_differ/dest/2.xlsx
+++ b/test/excel_differ/dest/2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\Python\gameff-toolset\test\excel_differ\dest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A718651-A4AF-4C64-94D2-EC0F4717471E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5B2D0D-FC8F-4B05-BFA2-8187D8C3E18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23748" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -742,24 +742,47 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>1998</v>
+      </c>
+      <c r="F11">
+        <v>888</v>
+      </c>
+      <c r="G11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>2003</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>546</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>13</v>
       </c>
     </row>

</xml_diff>